<commit_message>
Fixed exception throw from POI when not found sheet that definded in FileFormat
</commit_message>
<xml_diff>
--- a/src/main/resources/sampleReport.xlsx
+++ b/src/main/resources/sampleReport.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -491,28 +489,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new tag BeginRecordCondition for configure start data record dynamically
</commit_message>
<xml_diff>
--- a/src/main/resources/sampleReport.xlsx
+++ b/src/main/resources/sampleReport.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>As of</t>
   </si>
@@ -41,19 +41,36 @@
   </si>
   <si>
     <t>2014Jan01</t>
+  </si>
+  <si>
+    <t>sampleBegin</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>test date text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -65,7 +82,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,14 +90,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -170,7 +210,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -205,7 +244,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -381,21 +419,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="4" max="4" width="11.25" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -404,84 +443,107 @@
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="B5">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>100</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="B6">
+      <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>20.99</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="B7">
+      <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="B8">
+      <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9">
+      <c r="B9" s="5">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>50</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="E10" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E11" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed NullPointerException when <BeginRecordCondition/> not configured
</commit_message>
<xml_diff>
--- a/src/main/resources/sampleReport.xlsx
+++ b/src/main/resources/sampleReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>As of</t>
   </si>
@@ -50,13 +50,55 @@
   </si>
   <si>
     <t>test date text</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>fffff</t>
+  </si>
+  <si>
+    <t>gggg</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>ii</t>
+  </si>
+  <si>
+    <t>jjj</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>LLL</t>
+  </si>
+  <si>
+    <t>mmm</t>
+  </si>
+  <si>
+    <t>nn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +115,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -82,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -105,11 +154,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -121,6 +179,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E11"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -431,9 +495,15 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="4" max="4" width="11.25" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="1" spans="1:7">
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -446,8 +516,16 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G2" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="G3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
@@ -460,8 +538,11 @@
       <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="G4" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="B5" s="5">
         <v>1</v>
       </c>
@@ -474,8 +555,11 @@
       <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="G5" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="B6" s="5">
         <v>2</v>
       </c>
@@ -488,8 +572,11 @@
       <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="G6" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="B7" s="5">
         <v>3</v>
       </c>
@@ -500,8 +587,11 @@
       <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="G7" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="B8" s="5">
         <v>4</v>
       </c>
@@ -514,8 +604,11 @@
       <c r="E8" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="B9" s="5">
         <v>5</v>
       </c>
@@ -528,16 +621,22 @@
       <c r="E9" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="G9" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="4"/>
       <c r="E10" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G10" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
@@ -545,6 +644,24 @@
       <c r="D11" s="4"/>
       <c r="E11" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="G12" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="G13" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="G14" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>